<commit_message>
transformando los unicode restantes con utf16
</commit_message>
<xml_diff>
--- a/GrupLAC/Input/Base.xlsx
+++ b/GrupLAC/Input/Base.xlsx
@@ -554,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -562,6 +562,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -845,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1227,7 @@
       <c r="B34" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="7" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1441,8 +1442,9 @@
     <hyperlink ref="C11" r:id="rId9"/>
     <hyperlink ref="C12" r:id="rId10"/>
     <hyperlink ref="C10" r:id="rId11"/>
+    <hyperlink ref="C34" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>